<commit_message>
Added saving to excel, working on cleaning everything up!
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/Player_location.xlsx
+++ b/assets/spreadsheets/Player_location.xlsx
@@ -1,74 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jayden\PycharmProjects\pythonProject1\assets\spreadsheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BE018F-8917-4F5C-80F8-882F64199C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-360" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-360" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Player" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>player_x</t>
-  </si>
-  <si>
-    <t>player_y</t>
-  </si>
-  <si>
-    <t>player_image_x</t>
-  </si>
-  <si>
-    <t>player_image_y</t>
-  </si>
-  <si>
-    <t>camera_x</t>
-  </si>
-  <si>
-    <t>camera_y</t>
-  </si>
-  <si>
-    <t>current_room</t>
-  </si>
-  <si>
-    <t>Ringside</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <name val="Arial"/>
       <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <color theme="1"/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -87,23 +53,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -304,90 +329,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="4" width="21.28515625" customWidth="1"/>
+    <col width="21.28515625" customWidth="1" min="3" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>player_x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>player_y</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>player_image_x</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>player_image_y</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>camera_x</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>camera_y</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>current_room</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>79</v>
-      </c>
-      <c r="B2" s="2">
-        <v>79</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-79</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-79</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="E2" s="1" t="n">
+        <v>-101</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>-78</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Ringside</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>